<commit_message>
Update Formulaire de dépôt.xlsx
</commit_message>
<xml_diff>
--- a/Formulaire de dépôt.xlsx
+++ b/Formulaire de dépôt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\Documents\GitHub\FORT_BOYARD_SIMULATOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5DA478-13E0-43AD-8D16-42184DBDDCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55826106-AFDB-47DE-A247-74BA1B021C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8777C342-B2A2-AA44-A350-92F346BCACCE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>Critères</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>https://github.com/ranelden/FORT_BOYARD_SIMULATOR/</t>
+  </si>
+  <si>
+    <t>init, tour_navale, gagne_navale, jeu_bataille_navale, epreuve_logique, demande_position, affiche_grille_navale, grille_vide, suiv, jeu_tictactoe, tour_maitre_morpion, tour_joueur, coup_maitre,  grille_complete, verifier_victoire, affiche_grille_morpion, jeu_nim, maitre_retrait, joueur_retrait, affiche_batonnets</t>
   </si>
 </sst>
 </file>
@@ -756,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D512BAB-292A-D945-AF60-7F49E0D307FB}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" activeCellId="1" sqref="B18 C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75"/>
@@ -1011,7 +1014,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>38</v>
@@ -1364,6 +1367,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c236c89c-cb28-446f-abf1-caea36bbabb6">
@@ -1371,15 +1383,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1402,6 +1405,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D90C047-7704-4327-B6F5-04DA2C78DC65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F90BB40-EACC-4BE6-B342-3F14ABFB9970}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1416,12 +1427,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D90C047-7704-4327-B6F5-04DA2C78DC65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>